<commit_message>
försökt lägga till gpu i out :bug: och gated 4l resultat :rocket:
</commit_message>
<xml_diff>
--- a/Resultat/Resultat.xlsx
+++ b/Resultat/Resultat.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="79" documentId="11_0B75A8EC36B784AF83EBC3A6BB2527D4D88CE26C" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8CF9ECD4-BDAC-4787-B52C-BC80A7A2B188}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GATED" sheetId="1" r:id="rId1"/>
@@ -12,12 +13,45 @@
     <sheet name="GAT" sheetId="3" r:id="rId3"/>
     <sheet name="SAGE" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="43">
   <si>
     <t>SEED</t>
   </si>
@@ -86,16 +120,76 @@
   </si>
   <si>
     <t>P-norm, clamp(1,100),  batch_size: 32, Inget alpha</t>
+  </si>
+  <si>
+    <t>P-norm, 4 lager, clamp(1,100), batch_size = 128, p_init=rand()*6+1</t>
+  </si>
+  <si>
+    <t>85.6628</t>
+  </si>
+  <si>
+    <t>85.7851</t>
+  </si>
+  <si>
+    <t>1.8512</t>
+  </si>
+  <si>
+    <t>TOTAL TIME (h)</t>
+  </si>
+  <si>
+    <t>147.1467</t>
+  </si>
+  <si>
+    <t>EPOCH TIME (s)</t>
+  </si>
+  <si>
+    <t>P100-PCIE-16GB</t>
+  </si>
+  <si>
+    <t>85.6828</t>
+  </si>
+  <si>
+    <t>85.9627</t>
+  </si>
+  <si>
+    <t>3.1039</t>
+  </si>
+  <si>
+    <t>146.4936</t>
+  </si>
+  <si>
+    <t>85.7062</t>
+  </si>
+  <si>
+    <t>85.9406</t>
+  </si>
+  <si>
+    <t>146.7176</t>
+  </si>
+  <si>
+    <t>2.3349</t>
+  </si>
+  <si>
+    <t>85.7013</t>
+  </si>
+  <si>
+    <t>85.9425</t>
+  </si>
+  <si>
+    <t>2.1307</t>
+  </si>
+  <si>
+    <t>146.6605</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,6 +208,24 @@
       <color rgb="FFD4D4D4"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -142,19 +254,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,185 +587,188 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="26" name="Tabell2112427" displayName="Tabell2112427" ref="B3:J12" totalsRowShown="0" dataDxfId="99">
-  <autoFilter ref="B3:J12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabell2112427" displayName="Tabell2112427" ref="B4:J13" totalsRowShown="0" dataDxfId="99">
+  <autoFilter ref="B4:J13" xr:uid="{00000000-0009-0000-0100-00001A000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="SEED" dataDxfId="98"/>
-    <tableColumn id="12" name="Layers" dataDxfId="97"/>
-    <tableColumn id="10" name="Params" dataDxfId="96"/>
-    <tableColumn id="2" name="TEST_ACC" dataDxfId="95"/>
-    <tableColumn id="3" name="TRAIN_ACC" dataDxfId="94"/>
-    <tableColumn id="4" name="EPOCHS" dataDxfId="93"/>
-    <tableColumn id="5" name="EPOCH TIME" dataDxfId="92"/>
-    <tableColumn id="6" name="TOTAL TIME" dataDxfId="91"/>
-    <tableColumn id="11" name="GPU" dataDxfId="90"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="SEED" dataDxfId="98"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Layers" dataDxfId="97"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Params" dataDxfId="96"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="TEST_ACC" dataDxfId="95"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="TRAIN_ACC" dataDxfId="94"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="EPOCHS" dataDxfId="93"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="EPOCH TIME (s)" dataDxfId="92"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="TOTAL TIME (h)" dataDxfId="91"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="GPU" dataDxfId="90"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabell2112" displayName="Tabell2112" ref="B4:J11" totalsRowShown="0" dataDxfId="9">
-  <autoFilter ref="B4:J11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Tabell2112" displayName="Tabell2112" ref="B4:J11" totalsRowShown="0" dataDxfId="9">
+  <autoFilter ref="B4:J11" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="SEED" dataDxfId="8"/>
-    <tableColumn id="12" name="Layers" dataDxfId="7"/>
-    <tableColumn id="10" name="Params" dataDxfId="6"/>
-    <tableColumn id="2" name="TEST_ACC" dataDxfId="5"/>
-    <tableColumn id="3" name="TRAIN_ACC" dataDxfId="4"/>
-    <tableColumn id="4" name="EPOCHS" dataDxfId="3"/>
-    <tableColumn id="5" name="EPOCH TIME" dataDxfId="2"/>
-    <tableColumn id="6" name="TOTAL TIME" dataDxfId="1"/>
-    <tableColumn id="11" name="GPU" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="SEED" dataDxfId="8"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0900-00000C000000}" name="Layers" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0900-00000A000000}" name="Params" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="TEST_ACC" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="TRAIN_ACC" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="EPOCHS" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="EPOCH TIME" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0900-000006000000}" name="TOTAL TIME" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0900-00000B000000}" name="GPU" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="27" name="Tabell2112428" displayName="Tabell2112428" ref="B19:J28" totalsRowShown="0" dataDxfId="89">
-  <autoFilter ref="B19:J28"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="27" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabell2112428" displayName="Tabell2112428" ref="B20:J29" totalsRowShown="0" dataDxfId="89">
+  <autoFilter ref="B20:J29" xr:uid="{00000000-0009-0000-0100-00001B000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="SEED" dataDxfId="88"/>
-    <tableColumn id="12" name="Layers" dataDxfId="87"/>
-    <tableColumn id="10" name="Params" dataDxfId="86"/>
-    <tableColumn id="2" name="TEST_ACC" dataDxfId="85"/>
-    <tableColumn id="3" name="TRAIN_ACC" dataDxfId="84"/>
-    <tableColumn id="4" name="EPOCHS" dataDxfId="83"/>
-    <tableColumn id="5" name="EPOCH TIME" dataDxfId="82"/>
-    <tableColumn id="6" name="TOTAL TIME" dataDxfId="81"/>
-    <tableColumn id="11" name="GPU" dataDxfId="80"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="SEED" dataDxfId="88"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Layers" dataDxfId="87"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Params" dataDxfId="86"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="TEST_ACC" dataDxfId="85"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="TRAIN_ACC" dataDxfId="84"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="EPOCHS" dataDxfId="83"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="EPOCH TIME" dataDxfId="82"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="TOTAL TIME" dataDxfId="81"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="GPU" dataDxfId="80"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="28" name="Tabell2112429" displayName="Tabell2112429" ref="B35:J44" totalsRowShown="0" dataDxfId="79">
-  <autoFilter ref="B35:J44"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="28" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabell2112429" displayName="Tabell2112429" ref="B36:J45" totalsRowShown="0" dataDxfId="79">
+  <autoFilter ref="B36:J45" xr:uid="{00000000-0009-0000-0100-00001C000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="SEED" dataDxfId="78"/>
-    <tableColumn id="12" name="Layers" dataDxfId="77"/>
-    <tableColumn id="10" name="Params" dataDxfId="76"/>
-    <tableColumn id="2" name="TEST_ACC" dataDxfId="75"/>
-    <tableColumn id="3" name="TRAIN_ACC" dataDxfId="74"/>
-    <tableColumn id="4" name="EPOCHS" dataDxfId="73"/>
-    <tableColumn id="5" name="EPOCH TIME" dataDxfId="72"/>
-    <tableColumn id="6" name="TOTAL TIME" dataDxfId="71"/>
-    <tableColumn id="11" name="GPU" dataDxfId="70"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="SEED" dataDxfId="78"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Layers" dataDxfId="77"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="Params" dataDxfId="76"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="TEST_ACC" dataDxfId="75"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="TRAIN_ACC" dataDxfId="74"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="EPOCHS" dataDxfId="73"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="EPOCH TIME" dataDxfId="72"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="TOTAL TIME" dataDxfId="71"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="GPU" dataDxfId="70"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabell211" displayName="Tabell211" ref="B4:J11" totalsRowShown="0" dataDxfId="69">
-  <autoFilter ref="B4:J11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tabell211" displayName="Tabell211" ref="B4:J11" totalsRowShown="0" dataDxfId="69">
+  <autoFilter ref="B4:J11" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="SEED" dataDxfId="68"/>
-    <tableColumn id="12" name="Layers" dataDxfId="67"/>
-    <tableColumn id="10" name="Params" dataDxfId="66"/>
-    <tableColumn id="2" name="TEST_ACC" dataDxfId="65"/>
-    <tableColumn id="3" name="TRAIN_ACC" dataDxfId="64"/>
-    <tableColumn id="4" name="EPOCHS" dataDxfId="63"/>
-    <tableColumn id="5" name="EPOCH TIME" dataDxfId="62"/>
-    <tableColumn id="6" name="TOTAL TIME" dataDxfId="61"/>
-    <tableColumn id="11" name="GPU" dataDxfId="60"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="SEED" dataDxfId="68"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0300-00000C000000}" name="Layers" dataDxfId="67"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0300-00000A000000}" name="Params" dataDxfId="66"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="TEST_ACC" dataDxfId="65"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="TRAIN_ACC" dataDxfId="64"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="EPOCHS" dataDxfId="63"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="EPOCH TIME" dataDxfId="62"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="TOTAL TIME" dataDxfId="61"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0300-00000B000000}" name="GPU" dataDxfId="60"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="23" name="Tabell21124" displayName="Tabell21124" ref="B20:J29" totalsRowShown="0" dataDxfId="59">
-  <autoFilter ref="B20:J29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Tabell21124" displayName="Tabell21124" ref="B20:J29" totalsRowShown="0" dataDxfId="59">
+  <autoFilter ref="B20:J29" xr:uid="{00000000-0009-0000-0100-000017000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="SEED" dataDxfId="58"/>
-    <tableColumn id="12" name="Layers" dataDxfId="57"/>
-    <tableColumn id="10" name="Params" dataDxfId="56"/>
-    <tableColumn id="2" name="TEST_ACC" dataDxfId="55"/>
-    <tableColumn id="3" name="TRAIN_ACC" dataDxfId="54"/>
-    <tableColumn id="4" name="EPOCHS" dataDxfId="53"/>
-    <tableColumn id="5" name="EPOCH TIME" dataDxfId="52"/>
-    <tableColumn id="6" name="TOTAL TIME" dataDxfId="51"/>
-    <tableColumn id="11" name="GPU" dataDxfId="50"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="SEED" dataDxfId="58"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0400-00000C000000}" name="Layers" dataDxfId="57"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0400-00000A000000}" name="Params" dataDxfId="56"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="TEST_ACC" dataDxfId="55"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="TRAIN_ACC" dataDxfId="54"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="EPOCHS" dataDxfId="53"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="EPOCH TIME" dataDxfId="52"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="TOTAL TIME" dataDxfId="51"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0400-00000B000000}" name="GPU" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="25" name="Tabell2112426" displayName="Tabell2112426" ref="B36:J45" totalsRowShown="0" dataDxfId="49">
-  <autoFilter ref="B36:J45"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Tabell2112426" displayName="Tabell2112426" ref="B36:J45" totalsRowShown="0" dataDxfId="49">
+  <autoFilter ref="B36:J45" xr:uid="{00000000-0009-0000-0100-000019000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="SEED" dataDxfId="48"/>
-    <tableColumn id="12" name="Layers" dataDxfId="47"/>
-    <tableColumn id="10" name="Params" dataDxfId="46"/>
-    <tableColumn id="2" name="TEST_ACC" dataDxfId="45"/>
-    <tableColumn id="3" name="TRAIN_ACC" dataDxfId="44"/>
-    <tableColumn id="4" name="EPOCHS" dataDxfId="43"/>
-    <tableColumn id="5" name="EPOCH TIME" dataDxfId="42"/>
-    <tableColumn id="6" name="TOTAL TIME" dataDxfId="41"/>
-    <tableColumn id="11" name="GPU" dataDxfId="40"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="SEED" dataDxfId="48"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0500-00000C000000}" name="Layers" dataDxfId="47"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0500-00000A000000}" name="Params" dataDxfId="46"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="TEST_ACC" dataDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="TRAIN_ACC" dataDxfId="44"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="EPOCHS" dataDxfId="43"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="EPOCH TIME" dataDxfId="42"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="TOTAL TIME" dataDxfId="41"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0500-00000B000000}" name="GPU" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="29" name="Tabell2112430" displayName="Tabell2112430" ref="C5:K14" totalsRowShown="0" dataDxfId="39">
-  <autoFilter ref="C5:K14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="29" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Tabell2112430" displayName="Tabell2112430" ref="C5:K14" totalsRowShown="0" dataDxfId="39">
+  <autoFilter ref="C5:K14" xr:uid="{00000000-0009-0000-0100-00001D000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="SEED" dataDxfId="38"/>
-    <tableColumn id="12" name="Layers" dataDxfId="37"/>
-    <tableColumn id="10" name="Params" dataDxfId="36"/>
-    <tableColumn id="2" name="TEST_ACC" dataDxfId="35"/>
-    <tableColumn id="3" name="TRAIN_ACC" dataDxfId="34"/>
-    <tableColumn id="4" name="EPOCHS" dataDxfId="33"/>
-    <tableColumn id="5" name="EPOCH TIME" dataDxfId="32"/>
-    <tableColumn id="6" name="TOTAL TIME" dataDxfId="31"/>
-    <tableColumn id="11" name="GPU" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="SEED" dataDxfId="38"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0600-00000C000000}" name="Layers" dataDxfId="37"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0600-00000A000000}" name="Params" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="TEST_ACC" dataDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="TRAIN_ACC" dataDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="EPOCHS" dataDxfId="33"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="EPOCH TIME" dataDxfId="32"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="TOTAL TIME" dataDxfId="31"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0600-00000B000000}" name="GPU" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="30" name="Tabell2112431" displayName="Tabell2112431" ref="C21:K30" totalsRowShown="0" dataDxfId="29">
-  <autoFilter ref="C21:K30"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="30" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Tabell2112431" displayName="Tabell2112431" ref="C21:K30" totalsRowShown="0" dataDxfId="29">
+  <autoFilter ref="C21:K30" xr:uid="{00000000-0009-0000-0100-00001E000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="SEED" dataDxfId="28"/>
-    <tableColumn id="12" name="Layers" dataDxfId="27"/>
-    <tableColumn id="10" name="Params" dataDxfId="26"/>
-    <tableColumn id="2" name="TEST_ACC" dataDxfId="25"/>
-    <tableColumn id="3" name="TRAIN_ACC" dataDxfId="24"/>
-    <tableColumn id="4" name="EPOCHS" dataDxfId="23"/>
-    <tableColumn id="5" name="EPOCH TIME" dataDxfId="22"/>
-    <tableColumn id="6" name="TOTAL TIME" dataDxfId="21"/>
-    <tableColumn id="11" name="GPU" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="SEED" dataDxfId="28"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0700-00000C000000}" name="Layers" dataDxfId="27"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0700-00000A000000}" name="Params" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="TEST_ACC" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="TRAIN_ACC" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="EPOCHS" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="EPOCH TIME" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="TOTAL TIME" dataDxfId="21"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0700-00000B000000}" name="GPU" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="32" name="Tabell2112433" displayName="Tabell2112433" ref="C37:K46" totalsRowShown="0" dataDxfId="19">
-  <autoFilter ref="C37:K46"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="32" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Tabell2112433" displayName="Tabell2112433" ref="C37:K46" totalsRowShown="0" dataDxfId="19">
+  <autoFilter ref="C37:K46" xr:uid="{00000000-0009-0000-0100-000020000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="SEED" dataDxfId="18"/>
-    <tableColumn id="12" name="Layers" dataDxfId="17"/>
-    <tableColumn id="10" name="Params" dataDxfId="16"/>
-    <tableColumn id="2" name="TEST_ACC" dataDxfId="15"/>
-    <tableColumn id="3" name="TRAIN_ACC" dataDxfId="14"/>
-    <tableColumn id="4" name="EPOCHS" dataDxfId="13"/>
-    <tableColumn id="5" name="EPOCH TIME" dataDxfId="12"/>
-    <tableColumn id="6" name="TOTAL TIME" dataDxfId="11"/>
-    <tableColumn id="11" name="GPU" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="SEED" dataDxfId="18"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0800-00000C000000}" name="Layers" dataDxfId="17"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0800-00000A000000}" name="Params" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="TEST_ACC" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="TRAIN_ACC" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="EPOCHS" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="EPOCH TIME" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="TOTAL TIME" dataDxfId="11"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0800-00000B000000}" name="GPU" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -693,7 +817,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -726,9 +850,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -761,6 +902,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -936,122 +1094,183 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" customWidth="1"/>
-    <col min="10" max="10" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.73046875" customWidth="1"/>
+    <col min="3" max="3" width="15.1328125" customWidth="1"/>
+    <col min="4" max="4" width="12.1328125" customWidth="1"/>
+    <col min="5" max="5" width="15.73046875" customWidth="1"/>
+    <col min="6" max="6" width="18.265625" customWidth="1"/>
+    <col min="7" max="7" width="14.86328125" customWidth="1"/>
+    <col min="8" max="8" width="17.1328125" customWidth="1"/>
+    <col min="9" max="9" width="17.59765625" customWidth="1"/>
+    <col min="10" max="10" width="19.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" t="s">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F4" t="s">
         <v>2</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G4" t="s">
         <v>3</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B5" s="2">
+        <v>41</v>
+      </c>
+      <c r="C5" s="2">
         <v>4</v>
       </c>
-      <c r="I3" t="s">
-        <v>5</v>
-      </c>
-      <c r="J3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D5" s="6">
+        <v>104283</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="8">
+        <v>51</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B6" s="2">
+        <v>35</v>
+      </c>
+      <c r="C6" s="2">
+        <v>4</v>
+      </c>
+      <c r="D6" s="6">
+        <v>104283</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="8">
+        <v>56</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B7" s="2">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2">
+        <v>4</v>
+      </c>
+      <c r="D7" s="6">
+        <v>104283</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="8">
+        <v>75</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B8" s="2">
+        <v>95</v>
+      </c>
+      <c r="C8" s="2">
+        <v>4</v>
+      </c>
+      <c r="D8" s="6">
+        <v>104283</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="8">
+        <v>44</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -1062,7 +1281,7 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -1073,7 +1292,7 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -1084,7 +1303,567 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="e" cm="1">
+        <f t="array" ref="E12">MED</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F12" s="2" t="e">
+        <f>SUBTOTAL(101,F7:F10)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2" t="e">
+        <f>AVERAGE(E5:E8)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F13" s="2" t="e">
+        <f>STDEV(F7:F10)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" t="s">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>2</v>
+      </c>
+      <c r="G20" t="s">
+        <v>3</v>
+      </c>
+      <c r="H20" t="s">
+        <v>4</v>
+      </c>
+      <c r="I20" t="s">
+        <v>5</v>
+      </c>
+      <c r="J20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B35" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B36" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" t="s">
+        <v>1</v>
+      </c>
+      <c r="F36" t="s">
+        <v>2</v>
+      </c>
+      <c r="G36" t="s">
+        <v>3</v>
+      </c>
+      <c r="H36" t="s">
+        <v>4</v>
+      </c>
+      <c r="I36" t="s">
+        <v>5</v>
+      </c>
+      <c r="J36" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <tableParts count="3">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:N45"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="11.59765625" customWidth="1"/>
+    <col min="3" max="3" width="13.59765625" customWidth="1"/>
+    <col min="4" max="4" width="14.73046875" customWidth="1"/>
+    <col min="5" max="5" width="14.86328125" customWidth="1"/>
+    <col min="6" max="6" width="12.1328125" customWidth="1"/>
+    <col min="7" max="7" width="11.265625" customWidth="1"/>
+    <col min="8" max="8" width="13.59765625" customWidth="1"/>
+    <col min="9" max="9" width="19.86328125" customWidth="1"/>
+    <col min="10" max="10" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="B5" s="2">
+        <v>41</v>
+      </c>
+      <c r="C5" s="2">
+        <v>16</v>
+      </c>
+      <c r="D5" s="2">
+        <v>510558</v>
+      </c>
+      <c r="E5" s="3">
+        <v>85.503200000000007</v>
+      </c>
+      <c r="F5" s="2">
+        <v>86.014700000000005</v>
+      </c>
+      <c r="G5" s="2">
+        <v>63</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N5" s="1"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="B6" s="2">
+        <v>53</v>
+      </c>
+      <c r="C6" s="2">
+        <v>16</v>
+      </c>
+      <c r="D6" s="2">
+        <v>510558</v>
+      </c>
+      <c r="E6" s="3">
+        <v>85.5505</v>
+      </c>
+      <c r="F6" s="2">
+        <v>85.807299999999998</v>
+      </c>
+      <c r="G6" s="2">
+        <v>64</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="B7" s="2">
+        <v>76</v>
+      </c>
+      <c r="C7" s="2">
+        <v>16</v>
+      </c>
+      <c r="D7" s="2">
+        <v>510558</v>
+      </c>
+      <c r="E7" s="3">
+        <v>85.229299999999995</v>
+      </c>
+      <c r="F7" s="2">
+        <v>85.645899999999997</v>
+      </c>
+      <c r="G7" s="2">
+        <v>50</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="B8" s="2">
+        <v>12</v>
+      </c>
+      <c r="C8" s="2">
+        <v>16</v>
+      </c>
+      <c r="D8" s="2">
+        <v>510558</v>
+      </c>
+      <c r="E8" s="2">
+        <v>85.462599999999995</v>
+      </c>
+      <c r="F8" s="2">
+        <v>86.2697</v>
+      </c>
+      <c r="G8" s="2">
+        <v>48</v>
+      </c>
+      <c r="H8" s="2">
+        <v>566.55330000000004</v>
+      </c>
+      <c r="I8" s="2">
+        <v>27939.581600000001</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2">
+        <f>SUBTOTAL(101,E5:E8)</f>
+        <v>85.436400000000006</v>
+      </c>
+      <c r="F10" s="2">
+        <f>SUBTOTAL(101,F5:F8)</f>
+        <v>85.934399999999997</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2">
+        <f>STDEV(E5:E8)</f>
+        <v>0.14266265570686046</v>
+      </c>
+      <c r="F11" s="2">
+        <f>STDEV(F5:F8)</f>
+        <v>0.2697287773548353</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -1095,52 +1874,52 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B20" t="s">
         <v>0</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>15</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D20" t="s">
         <v>9</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E20" t="s">
         <v>1</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F20" t="s">
         <v>2</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G20" t="s">
         <v>3</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H20" t="s">
         <v>4</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I20" t="s">
         <v>5</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -1151,7 +1930,7 @@
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -1162,7 +1941,7 @@
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -1173,7 +1952,7 @@
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -1184,7 +1963,7 @@
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -1195,7 +1974,7 @@
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -1206,7 +1985,7 @@
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -1217,7 +1996,7 @@
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -1228,52 +2007,52 @@
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B36" t="s">
         <v>0</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>15</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D36" t="s">
         <v>9</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E36" t="s">
         <v>1</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F36" t="s">
         <v>2</v>
       </c>
-      <c r="G35" t="s">
+      <c r="G36" t="s">
         <v>3</v>
       </c>
-      <c r="H35" t="s">
+      <c r="H36" t="s">
         <v>4</v>
       </c>
-      <c r="I35" t="s">
+      <c r="I36" t="s">
         <v>5</v>
       </c>
-      <c r="J35" t="s">
+      <c r="J36" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -1284,7 +2063,7 @@
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -1295,7 +2074,7 @@
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -1306,7 +2085,7 @@
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -1317,7 +2096,7 @@
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -1328,7 +2107,7 @@
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -1339,7 +2118,7 @@
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -1350,7 +2129,7 @@
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -1361,540 +2140,7 @@
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="3">
-    <tablePart r:id="rId1"/>
-    <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N45"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:J11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" customWidth="1"/>
-    <col min="9" max="9" width="19.85546875" customWidth="1"/>
-    <col min="10" max="10" width="18" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="2">
-        <v>41</v>
-      </c>
-      <c r="C5" s="2">
-        <v>16</v>
-      </c>
-      <c r="D5" s="2">
-        <v>510558</v>
-      </c>
-      <c r="E5" s="3">
-        <v>85.503200000000007</v>
-      </c>
-      <c r="F5" s="2">
-        <v>86.014700000000005</v>
-      </c>
-      <c r="G5" s="2">
-        <v>63</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N5" s="1"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="2">
-        <v>53</v>
-      </c>
-      <c r="C6" s="2">
-        <v>16</v>
-      </c>
-      <c r="D6" s="2">
-        <v>510558</v>
-      </c>
-      <c r="E6" s="3">
-        <v>85.5505</v>
-      </c>
-      <c r="F6" s="2">
-        <v>85.807299999999998</v>
-      </c>
-      <c r="G6" s="2">
-        <v>64</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="2">
-        <v>76</v>
-      </c>
-      <c r="C7" s="2">
-        <v>16</v>
-      </c>
-      <c r="D7" s="2">
-        <v>510558</v>
-      </c>
-      <c r="E7" s="3">
-        <v>85.229299999999995</v>
-      </c>
-      <c r="F7" s="2">
-        <v>85.645899999999997</v>
-      </c>
-      <c r="G7" s="2">
-        <v>50</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="2">
-        <v>12</v>
-      </c>
-      <c r="C8" s="2">
-        <v>16</v>
-      </c>
-      <c r="D8" s="2">
-        <v>510558</v>
-      </c>
-      <c r="E8" s="2">
-        <v>85.462599999999995</v>
-      </c>
-      <c r="F8" s="2">
-        <v>86.2697</v>
-      </c>
-      <c r="G8" s="2">
-        <v>48</v>
-      </c>
-      <c r="H8" s="2">
-        <v>566.55330000000004</v>
-      </c>
-      <c r="I8" s="2">
-        <v>27939.581600000001</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2">
-        <f>SUBTOTAL(101,E5:E8)</f>
-        <v>85.436400000000006</v>
-      </c>
-      <c r="F10" s="2">
-        <f>SUBTOTAL(101,F5:F8)</f>
-        <v>85.934399999999997</v>
-      </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2">
-        <f>STDEV(E5:E8)</f>
-        <v>0.14266265570686046</v>
-      </c>
-      <c r="F11" s="2">
-        <f>STDEV(F5:F8)</f>
-        <v>0.2697287773548353</v>
-      </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" t="s">
-        <v>1</v>
-      </c>
-      <c r="F20" t="s">
-        <v>2</v>
-      </c>
-      <c r="G20" t="s">
-        <v>3</v>
-      </c>
-      <c r="H20" t="s">
-        <v>4</v>
-      </c>
-      <c r="I20" t="s">
-        <v>5</v>
-      </c>
-      <c r="J20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>0</v>
-      </c>
-      <c r="C36" t="s">
-        <v>15</v>
-      </c>
-      <c r="D36" t="s">
-        <v>9</v>
-      </c>
-      <c r="E36" t="s">
-        <v>1</v>
-      </c>
-      <c r="F36" t="s">
-        <v>2</v>
-      </c>
-      <c r="G36" t="s">
-        <v>3</v>
-      </c>
-      <c r="H36" t="s">
-        <v>4</v>
-      </c>
-      <c r="I36" t="s">
-        <v>5</v>
-      </c>
-      <c r="J36" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
-    </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-    </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
-    </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
-    </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -1917,21 +2163,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="C4:K46"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="C37" sqref="C37:K46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="4" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C5" t="s">
         <v>0</v>
       </c>
@@ -1960,7 +2206,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -1971,7 +2217,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -1982,7 +2228,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -1993,7 +2239,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -2004,7 +2250,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -2015,7 +2261,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -2026,7 +2272,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -2037,7 +2283,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -2048,7 +2294,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -2059,12 +2305,12 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C20" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C21" t="s">
         <v>0</v>
       </c>
@@ -2093,7 +2339,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -2104,7 +2350,7 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -2115,7 +2361,7 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -2126,7 +2372,7 @@
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -2137,7 +2383,7 @@
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -2148,7 +2394,7 @@
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -2159,7 +2405,7 @@
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -2170,7 +2416,7 @@
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
     </row>
-    <row r="29" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -2181,7 +2427,7 @@
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -2192,12 +2438,12 @@
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
     </row>
-    <row r="36" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C36" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C37" t="s">
         <v>0</v>
       </c>
@@ -2226,7 +2472,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -2237,7 +2483,7 @@
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
     </row>
-    <row r="39" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -2248,7 +2494,7 @@
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
     </row>
-    <row r="40" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -2259,7 +2505,7 @@
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
     </row>
-    <row r="41" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -2270,7 +2516,7 @@
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
     </row>
-    <row r="42" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -2281,7 +2527,7 @@
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
     </row>
-    <row r="43" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -2292,7 +2538,7 @@
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
     </row>
-    <row r="44" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -2303,7 +2549,7 @@
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
     </row>
-    <row r="45" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -2314,7 +2560,7 @@
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
     </row>
-    <row r="46" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
@@ -2336,26 +2582,26 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="11.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" customWidth="1"/>
-    <col min="10" max="10" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.265625" customWidth="1"/>
+    <col min="4" max="4" width="12.73046875" customWidth="1"/>
+    <col min="5" max="5" width="14.265625" customWidth="1"/>
+    <col min="6" max="6" width="13.1328125" customWidth="1"/>
+    <col min="7" max="7" width="10.59765625" customWidth="1"/>
+    <col min="8" max="8" width="15.3984375" customWidth="1"/>
+    <col min="9" max="9" width="13.73046875" customWidth="1"/>
+    <col min="10" max="10" width="17.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
         <v>12</v>
       </c>
@@ -2382,16 +2628,16 @@
       </c>
       <c r="L1" s="5"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="L2" s="5"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>22</v>
       </c>
       <c r="L3" s="5"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -2421,7 +2667,7 @@
       </c>
       <c r="L4" s="5"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B5" s="2">
         <v>41</v>
       </c>
@@ -2436,7 +2682,7 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B6" s="2">
         <v>95</v>
       </c>
@@ -2451,7 +2697,7 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B7" s="2">
         <v>12</v>
       </c>
@@ -2466,7 +2712,7 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B8" s="2">
         <v>35</v>
       </c>
@@ -2481,7 +2727,7 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -2492,7 +2738,7 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="s">
         <v>21</v>
       </c>
@@ -2512,7 +2758,7 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -2529,7 +2775,7 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -2540,7 +2786,7 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -2551,7 +2797,7 @@
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -2562,7 +2808,7 @@
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -2573,7 +2819,7 @@
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -2584,7 +2830,7 @@
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -2595,7 +2841,7 @@
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -2606,7 +2852,7 @@
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -2617,7 +2863,7 @@
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -2628,7 +2874,7 @@
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -2639,7 +2885,7 @@
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -2650,7 +2896,7 @@
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -2661,7 +2907,7 @@
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -2672,7 +2918,7 @@
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -2683,7 +2929,7 @@
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -2694,7 +2940,7 @@
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -2705,7 +2951,7 @@
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -2716,7 +2962,7 @@
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -2727,7 +2973,7 @@
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>

</xml_diff>

<commit_message>
fix config n more :mushroom:
</commit_message>
<xml_diff>
--- a/Resultat/Resultat.xlsx
+++ b/Resultat/Resultat.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="79" documentId="11_0B75A8EC36B784AF83EBC3A6BB2527D4D88CE26C" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8CF9ECD4-BDAC-4787-B52C-BC80A7A2B188}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B57BB13-D3E7-4252-AD74-C6A70A1B9ABC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5970" yWindow="1890" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GATED" sheetId="1" r:id="rId1"/>
@@ -28,30 +28,8 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="35">
   <si>
     <t>SEED</t>
   </si>
@@ -125,12 +103,6 @@
     <t>P-norm, 4 lager, clamp(1,100), batch_size = 128, p_init=rand()*6+1</t>
   </si>
   <si>
-    <t>85.6628</t>
-  </si>
-  <si>
-    <t>85.7851</t>
-  </si>
-  <si>
     <t>1.8512</t>
   </si>
   <si>
@@ -146,34 +118,16 @@
     <t>P100-PCIE-16GB</t>
   </si>
   <si>
-    <t>85.6828</t>
-  </si>
-  <si>
-    <t>85.9627</t>
-  </si>
-  <si>
     <t>3.1039</t>
   </si>
   <si>
     <t>146.4936</t>
   </si>
   <si>
-    <t>85.7062</t>
-  </si>
-  <si>
-    <t>85.9406</t>
-  </si>
-  <si>
     <t>146.7176</t>
   </si>
   <si>
     <t>2.3349</t>
-  </si>
-  <si>
-    <t>85.7013</t>
-  </si>
-  <si>
-    <t>85.9425</t>
   </si>
   <si>
     <t>2.1307</t>
@@ -189,7 +143,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,20 +164,14 @@
       <family val="3"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -254,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -267,48 +215,164 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="100">
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
+  <dxfs count="101">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+      </font>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -595,180 +659,180 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabell2112427" displayName="Tabell2112427" ref="B4:J13" totalsRowShown="0" dataDxfId="99">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabell2112427" displayName="Tabell2112427" ref="B4:J13" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
   <autoFilter ref="B4:J13" xr:uid="{00000000-0009-0000-0100-00001A000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="SEED" dataDxfId="98"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Layers" dataDxfId="97"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Params" dataDxfId="96"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="TEST_ACC" dataDxfId="95"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="TRAIN_ACC" dataDxfId="94"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="EPOCHS" dataDxfId="93"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="EPOCH TIME (s)" dataDxfId="92"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="TOTAL TIME (h)" dataDxfId="91"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="GPU" dataDxfId="90"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="SEED" dataDxfId="10"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Layers" dataDxfId="9"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Params" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="TEST_ACC" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="TRAIN_ACC" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="EPOCHS" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="EPOCH TIME (s)" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="TOTAL TIME (h)" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="GPU" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Tabell2112" displayName="Tabell2112" ref="B4:J11" totalsRowShown="0" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Tabell2112" displayName="Tabell2112" ref="B4:J11" totalsRowShown="0" dataDxfId="20">
   <autoFilter ref="B4:J11" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="SEED" dataDxfId="8"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0900-00000C000000}" name="Layers" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0900-00000A000000}" name="Params" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="TEST_ACC" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="TRAIN_ACC" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="EPOCHS" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="EPOCH TIME" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0900-000006000000}" name="TOTAL TIME" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0900-00000B000000}" name="GPU" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="SEED" dataDxfId="19"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0900-00000C000000}" name="Layers" dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0900-00000A000000}" name="Params" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="TEST_ACC" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="TRAIN_ACC" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="EPOCHS" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="EPOCH TIME" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0900-000006000000}" name="TOTAL TIME" dataDxfId="12"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0900-00000B000000}" name="GPU" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="27" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabell2112428" displayName="Tabell2112428" ref="B20:J29" totalsRowShown="0" dataDxfId="89">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="27" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabell2112428" displayName="Tabell2112428" ref="B20:J29" totalsRowShown="0" dataDxfId="100">
   <autoFilter ref="B20:J29" xr:uid="{00000000-0009-0000-0100-00001B000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="SEED" dataDxfId="88"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Layers" dataDxfId="87"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Params" dataDxfId="86"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="TEST_ACC" dataDxfId="85"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="TRAIN_ACC" dataDxfId="84"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="EPOCHS" dataDxfId="83"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="EPOCH TIME" dataDxfId="82"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="TOTAL TIME" dataDxfId="81"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="GPU" dataDxfId="80"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="SEED" dataDxfId="99"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Layers" dataDxfId="98"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Params" dataDxfId="97"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="TEST_ACC" dataDxfId="96"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="TRAIN_ACC" dataDxfId="95"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="EPOCHS" dataDxfId="94"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="EPOCH TIME" dataDxfId="93"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="TOTAL TIME" dataDxfId="92"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="GPU" dataDxfId="91"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="28" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabell2112429" displayName="Tabell2112429" ref="B36:J45" totalsRowShown="0" dataDxfId="79">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="28" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabell2112429" displayName="Tabell2112429" ref="B36:J45" totalsRowShown="0" dataDxfId="90">
   <autoFilter ref="B36:J45" xr:uid="{00000000-0009-0000-0100-00001C000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="SEED" dataDxfId="78"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Layers" dataDxfId="77"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="Params" dataDxfId="76"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="TEST_ACC" dataDxfId="75"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="TRAIN_ACC" dataDxfId="74"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="EPOCHS" dataDxfId="73"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="EPOCH TIME" dataDxfId="72"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="TOTAL TIME" dataDxfId="71"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="GPU" dataDxfId="70"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="SEED" dataDxfId="89"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Layers" dataDxfId="88"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="Params" dataDxfId="87"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="TEST_ACC" dataDxfId="86"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="TRAIN_ACC" dataDxfId="85"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="EPOCHS" dataDxfId="84"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="EPOCH TIME" dataDxfId="83"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="TOTAL TIME" dataDxfId="82"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="GPU" dataDxfId="81"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tabell211" displayName="Tabell211" ref="B4:J11" totalsRowShown="0" dataDxfId="69">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tabell211" displayName="Tabell211" ref="B4:J11" totalsRowShown="0" dataDxfId="80">
   <autoFilter ref="B4:J11" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="SEED" dataDxfId="68"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0300-00000C000000}" name="Layers" dataDxfId="67"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0300-00000A000000}" name="Params" dataDxfId="66"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="TEST_ACC" dataDxfId="65"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="TRAIN_ACC" dataDxfId="64"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="EPOCHS" dataDxfId="63"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="EPOCH TIME" dataDxfId="62"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="TOTAL TIME" dataDxfId="61"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0300-00000B000000}" name="GPU" dataDxfId="60"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="SEED" dataDxfId="79"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0300-00000C000000}" name="Layers" dataDxfId="78"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0300-00000A000000}" name="Params" dataDxfId="77"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="TEST_ACC" dataDxfId="76"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="TRAIN_ACC" dataDxfId="75"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="EPOCHS" dataDxfId="74"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="EPOCH TIME" dataDxfId="73"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="TOTAL TIME" dataDxfId="72"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0300-00000B000000}" name="GPU" dataDxfId="71"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Tabell21124" displayName="Tabell21124" ref="B20:J29" totalsRowShown="0" dataDxfId="59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Tabell21124" displayName="Tabell21124" ref="B20:J29" totalsRowShown="0" dataDxfId="70">
   <autoFilter ref="B20:J29" xr:uid="{00000000-0009-0000-0100-000017000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="SEED" dataDxfId="58"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0400-00000C000000}" name="Layers" dataDxfId="57"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0400-00000A000000}" name="Params" dataDxfId="56"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="TEST_ACC" dataDxfId="55"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="TRAIN_ACC" dataDxfId="54"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="EPOCHS" dataDxfId="53"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="EPOCH TIME" dataDxfId="52"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="TOTAL TIME" dataDxfId="51"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0400-00000B000000}" name="GPU" dataDxfId="50"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="SEED" dataDxfId="69"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0400-00000C000000}" name="Layers" dataDxfId="68"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0400-00000A000000}" name="Params" dataDxfId="67"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="TEST_ACC" dataDxfId="66"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="TRAIN_ACC" dataDxfId="65"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="EPOCHS" dataDxfId="64"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="EPOCH TIME" dataDxfId="63"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="TOTAL TIME" dataDxfId="62"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0400-00000B000000}" name="GPU" dataDxfId="61"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Tabell2112426" displayName="Tabell2112426" ref="B36:J45" totalsRowShown="0" dataDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Tabell2112426" displayName="Tabell2112426" ref="B36:J45" totalsRowShown="0" dataDxfId="60">
   <autoFilter ref="B36:J45" xr:uid="{00000000-0009-0000-0100-000019000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="SEED" dataDxfId="48"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0500-00000C000000}" name="Layers" dataDxfId="47"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0500-00000A000000}" name="Params" dataDxfId="46"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="TEST_ACC" dataDxfId="45"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="TRAIN_ACC" dataDxfId="44"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="EPOCHS" dataDxfId="43"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="EPOCH TIME" dataDxfId="42"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="TOTAL TIME" dataDxfId="41"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0500-00000B000000}" name="GPU" dataDxfId="40"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="SEED" dataDxfId="59"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0500-00000C000000}" name="Layers" dataDxfId="58"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0500-00000A000000}" name="Params" dataDxfId="57"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="TEST_ACC" dataDxfId="56"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="TRAIN_ACC" dataDxfId="55"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="EPOCHS" dataDxfId="54"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="EPOCH TIME" dataDxfId="53"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="TOTAL TIME" dataDxfId="52"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0500-00000B000000}" name="GPU" dataDxfId="51"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="29" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Tabell2112430" displayName="Tabell2112430" ref="C5:K14" totalsRowShown="0" dataDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="29" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Tabell2112430" displayName="Tabell2112430" ref="C5:K14" totalsRowShown="0" dataDxfId="50">
   <autoFilter ref="C5:K14" xr:uid="{00000000-0009-0000-0100-00001D000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="SEED" dataDxfId="38"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0600-00000C000000}" name="Layers" dataDxfId="37"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0600-00000A000000}" name="Params" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="TEST_ACC" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="TRAIN_ACC" dataDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="EPOCHS" dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="EPOCH TIME" dataDxfId="32"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="TOTAL TIME" dataDxfId="31"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0600-00000B000000}" name="GPU" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="SEED" dataDxfId="49"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0600-00000C000000}" name="Layers" dataDxfId="48"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0600-00000A000000}" name="Params" dataDxfId="47"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="TEST_ACC" dataDxfId="46"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="TRAIN_ACC" dataDxfId="45"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="EPOCHS" dataDxfId="44"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="EPOCH TIME" dataDxfId="43"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="TOTAL TIME" dataDxfId="42"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0600-00000B000000}" name="GPU" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="30" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Tabell2112431" displayName="Tabell2112431" ref="C21:K30" totalsRowShown="0" dataDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="30" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Tabell2112431" displayName="Tabell2112431" ref="C21:K30" totalsRowShown="0" dataDxfId="40">
   <autoFilter ref="C21:K30" xr:uid="{00000000-0009-0000-0100-00001E000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="SEED" dataDxfId="28"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0700-00000C000000}" name="Layers" dataDxfId="27"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0700-00000A000000}" name="Params" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="TEST_ACC" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="TRAIN_ACC" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="EPOCHS" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="EPOCH TIME" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="TOTAL TIME" dataDxfId="21"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0700-00000B000000}" name="GPU" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="SEED" dataDxfId="39"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0700-00000C000000}" name="Layers" dataDxfId="38"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0700-00000A000000}" name="Params" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="TEST_ACC" dataDxfId="36"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="TRAIN_ACC" dataDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="EPOCHS" dataDxfId="34"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="EPOCH TIME" dataDxfId="33"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="TOTAL TIME" dataDxfId="32"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0700-00000B000000}" name="GPU" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="32" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Tabell2112433" displayName="Tabell2112433" ref="C37:K46" totalsRowShown="0" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="32" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Tabell2112433" displayName="Tabell2112433" ref="C37:K46" totalsRowShown="0" dataDxfId="30">
   <autoFilter ref="C37:K46" xr:uid="{00000000-0009-0000-0100-000020000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="SEED" dataDxfId="18"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0800-00000C000000}" name="Layers" dataDxfId="17"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0800-00000A000000}" name="Params" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="TEST_ACC" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="TRAIN_ACC" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="EPOCHS" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="EPOCH TIME" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="TOTAL TIME" dataDxfId="11"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0800-00000B000000}" name="GPU" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="SEED" dataDxfId="29"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0800-00000C000000}" name="Layers" dataDxfId="28"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0800-00000A000000}" name="Params" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="TEST_ACC" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="TRAIN_ACC" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="EPOCHS" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="EPOCH TIME" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="TOTAL TIME" dataDxfId="22"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0800-00000B000000}" name="GPU" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1097,255 +1161,255 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="13.73046875" customWidth="1"/>
-    <col min="3" max="3" width="15.1328125" customWidth="1"/>
-    <col min="4" max="4" width="12.1328125" customWidth="1"/>
-    <col min="5" max="5" width="15.73046875" customWidth="1"/>
-    <col min="6" max="6" width="18.265625" customWidth="1"/>
-    <col min="7" max="7" width="14.86328125" customWidth="1"/>
-    <col min="8" max="8" width="17.1328125" customWidth="1"/>
-    <col min="9" max="9" width="17.59765625" customWidth="1"/>
-    <col min="10" max="10" width="19.59765625" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" customWidth="1"/>
+    <col min="10" max="10" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="B4" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="7">
+        <v>41</v>
+      </c>
+      <c r="C5" s="7">
+        <v>4</v>
+      </c>
+      <c r="D5" s="8">
+        <v>104283</v>
+      </c>
+      <c r="E5" s="10">
+        <v>85.701300000000003</v>
+      </c>
+      <c r="F5" s="10">
+        <v>85.942499999999995</v>
+      </c>
+      <c r="G5" s="9">
+        <v>51</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="7">
+        <v>35</v>
+      </c>
+      <c r="C6" s="7">
+        <v>4</v>
+      </c>
+      <c r="D6" s="8">
+        <v>104283</v>
+      </c>
+      <c r="E6" s="10">
+        <v>85.706199999999995</v>
+      </c>
+      <c r="F6" s="10">
+        <v>85.940600000000003</v>
+      </c>
+      <c r="G6" s="9">
+        <v>56</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="7">
+        <v>12</v>
+      </c>
+      <c r="C7" s="7">
+        <v>4</v>
+      </c>
+      <c r="D7" s="8">
+        <v>104283</v>
+      </c>
+      <c r="E7" s="10">
+        <v>85.6828</v>
+      </c>
+      <c r="F7" s="10">
+        <v>85.962699999999998</v>
+      </c>
+      <c r="G7" s="9">
+        <v>75</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="I4" t="s">
-        <v>27</v>
-      </c>
-      <c r="J4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="B5" s="2">
-        <v>41</v>
-      </c>
-      <c r="C5" s="2">
+      <c r="J7" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="7">
+        <v>95</v>
+      </c>
+      <c r="C8" s="7">
         <v>4</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D8" s="8">
         <v>104283</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G5" s="8">
-        <v>51</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="B6" s="2">
-        <v>35</v>
-      </c>
-      <c r="C6" s="2">
-        <v>4</v>
-      </c>
-      <c r="D6" s="6">
-        <v>104283</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" s="8">
-        <v>56</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="B7" s="2">
-        <v>12</v>
-      </c>
-      <c r="C7" s="2">
-        <v>4</v>
-      </c>
-      <c r="D7" s="6">
-        <v>104283</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="G7" s="8">
-        <v>75</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="B8" s="2">
-        <v>95</v>
-      </c>
-      <c r="C8" s="2">
-        <v>4</v>
-      </c>
-      <c r="D8" s="6">
-        <v>104283</v>
-      </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="10">
+        <v>85.662800000000004</v>
+      </c>
+      <c r="F8" s="10">
+        <v>85.7851</v>
+      </c>
+      <c r="G8" s="9">
+        <v>44</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="8">
-        <v>44</v>
-      </c>
-      <c r="H8" s="6" t="s">
+      <c r="J8" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2" t="e" cm="1">
-        <f t="array" ref="E12">MED</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F12" s="2" t="e">
-        <f>SUBTOTAL(101,F7:F10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2" t="e">
-        <f>AVERAGE(E5:E8)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F13" s="2" t="e">
-        <f>STDEV(F7:F10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7">
+        <f>SUBTOTAL(101,E5:E8)</f>
+        <v>85.688275000000004</v>
+      </c>
+      <c r="F12" s="7">
+        <f>SUBTOTAL(101,F5:F8)</f>
+        <v>85.907724999999999</v>
+      </c>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7">
+        <f>STDEV(E5:E8)</f>
+        <v>1.9747636989436695E-2</v>
+      </c>
+      <c r="F13" s="7">
+        <f>STDEV(F5:F8)</f>
+        <v>8.2359390276194822E-2</v>
+      </c>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>0</v>
       </c>
@@ -1374,7 +1438,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -1385,7 +1449,7 @@
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -1396,7 +1460,7 @@
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -1407,7 +1471,7 @@
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -1418,7 +1482,7 @@
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -1429,7 +1493,7 @@
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -1440,7 +1504,7 @@
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -1451,7 +1515,7 @@
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -1462,7 +1526,7 @@
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -1473,12 +1537,12 @@
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>0</v>
       </c>
@@ -1507,7 +1571,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -1518,7 +1582,7 @@
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -1529,7 +1593,7 @@
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -1540,7 +1604,7 @@
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -1551,7 +1615,7 @@
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -1562,7 +1626,7 @@
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -1573,7 +1637,7 @@
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -1584,7 +1648,7 @@
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -1595,7 +1659,7 @@
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -1622,23 +1686,23 @@
   <dimension ref="A1:N45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.59765625" customWidth="1"/>
-    <col min="3" max="3" width="13.59765625" customWidth="1"/>
-    <col min="4" max="4" width="14.73046875" customWidth="1"/>
-    <col min="5" max="5" width="14.86328125" customWidth="1"/>
-    <col min="6" max="6" width="12.1328125" customWidth="1"/>
-    <col min="7" max="7" width="11.265625" customWidth="1"/>
-    <col min="8" max="8" width="13.59765625" customWidth="1"/>
-    <col min="9" max="9" width="19.86328125" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" customWidth="1"/>
     <col min="10" max="10" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>12</v>
       </c>
@@ -1664,12 +1728,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -1698,7 +1762,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>41</v>
       </c>
@@ -1728,7 +1792,7 @@
       </c>
       <c r="N5" s="1"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>53</v>
       </c>
@@ -1757,7 +1821,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>76</v>
       </c>
@@ -1786,7 +1850,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>12</v>
       </c>
@@ -1815,7 +1879,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -1826,7 +1890,7 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>21</v>
       </c>
@@ -1846,7 +1910,7 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -1863,7 +1927,7 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -1874,7 +1938,7 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -1885,12 +1949,12 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>0</v>
       </c>
@@ -1919,7 +1983,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -1930,7 +1994,7 @@
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -1941,7 +2005,7 @@
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -1952,7 +2016,7 @@
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -1963,7 +2027,7 @@
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -1974,7 +2038,7 @@
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -1985,7 +2049,7 @@
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -1996,7 +2060,7 @@
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -2007,7 +2071,7 @@
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -2018,12 +2082,12 @@
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>0</v>
       </c>
@@ -2052,7 +2116,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -2063,7 +2127,7 @@
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -2074,7 +2138,7 @@
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -2085,7 +2149,7 @@
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -2096,7 +2160,7 @@
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -2107,7 +2171,7 @@
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -2118,7 +2182,7 @@
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -2129,7 +2193,7 @@
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -2140,7 +2204,7 @@
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -2170,14 +2234,14 @@
       <selection activeCell="C37" sqref="C37:K46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>0</v>
       </c>
@@ -2206,7 +2270,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -2217,7 +2281,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -2228,7 +2292,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -2239,7 +2303,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="9" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -2250,7 +2314,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -2261,7 +2325,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="11" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -2272,7 +2336,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -2283,7 +2347,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -2294,7 +2358,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="14" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -2305,12 +2369,12 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="20" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>0</v>
       </c>
@@ -2339,7 +2403,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="22" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -2350,7 +2414,7 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="23" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -2361,7 +2425,7 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -2372,7 +2436,7 @@
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="25" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -2383,7 +2447,7 @@
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="26" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -2394,7 +2458,7 @@
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="27" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -2405,7 +2469,7 @@
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="28" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -2416,7 +2480,7 @@
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
     </row>
-    <row r="29" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="29" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -2427,7 +2491,7 @@
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="30" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -2438,12 +2502,12 @@
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
     </row>
-    <row r="36" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="36" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="37" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
         <v>0</v>
       </c>
@@ -2472,7 +2536,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="38" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -2483,7 +2547,7 @@
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
     </row>
-    <row r="39" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="39" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -2494,7 +2558,7 @@
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
     </row>
-    <row r="40" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="40" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -2505,7 +2569,7 @@
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
     </row>
-    <row r="41" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="41" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -2516,7 +2580,7 @@
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
     </row>
-    <row r="42" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="42" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -2527,7 +2591,7 @@
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
     </row>
-    <row r="43" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="43" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -2538,7 +2602,7 @@
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
     </row>
-    <row r="44" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="44" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -2549,7 +2613,7 @@
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
     </row>
-    <row r="45" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="45" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -2560,7 +2624,7 @@
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
     </row>
-    <row r="46" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="46" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
@@ -2585,23 +2649,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.265625" customWidth="1"/>
-    <col min="4" max="4" width="12.73046875" customWidth="1"/>
-    <col min="5" max="5" width="14.265625" customWidth="1"/>
-    <col min="6" max="6" width="13.1328125" customWidth="1"/>
-    <col min="7" max="7" width="10.59765625" customWidth="1"/>
-    <col min="8" max="8" width="15.3984375" customWidth="1"/>
-    <col min="9" max="9" width="13.73046875" customWidth="1"/>
-    <col min="10" max="10" width="17.1328125" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="10" max="10" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>12</v>
       </c>
@@ -2628,16 +2692,16 @@
       </c>
       <c r="L1" s="5"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L2" s="5"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>22</v>
       </c>
       <c r="L3" s="5"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -2667,37 +2731,65 @@
       </c>
       <c r="L4" s="5"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>41</v>
       </c>
       <c r="C5" s="2">
         <v>4</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="D5" s="2">
+        <v>102095</v>
+      </c>
+      <c r="E5" s="3">
+        <v>85.742000000000004</v>
+      </c>
+      <c r="F5" s="2">
+        <v>86.226100000000002</v>
+      </c>
+      <c r="G5" s="2">
+        <v>71</v>
+      </c>
+      <c r="H5" s="2">
+        <v>126.459</v>
+      </c>
+      <c r="I5" s="2">
+        <v>9155.3444999999992</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>95</v>
       </c>
       <c r="C6" s="2">
         <v>4</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="D6" s="2">
+        <v>102095</v>
+      </c>
+      <c r="E6" s="3">
+        <v>85.761200000000002</v>
+      </c>
+      <c r="F6" s="2">
+        <v>86.037700000000001</v>
+      </c>
+      <c r="G6" s="2">
+        <v>62</v>
+      </c>
+      <c r="H6" s="2">
+        <v>126.9375</v>
+      </c>
+      <c r="I6" s="2">
+        <v>8047.9236000000001</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>12</v>
       </c>
@@ -2712,7 +2804,7 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>35</v>
       </c>
@@ -2727,7 +2819,7 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -2738,44 +2830,44 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="2" t="e">
+      <c r="E10" s="2">
         <f>SUBTOTAL(101,E5:E8)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F10" s="2" t="e">
+        <v>85.751599999999996</v>
+      </c>
+      <c r="F10" s="2">
         <f>SUBTOTAL(101,F5:F8)</f>
-        <v>#DIV/0!</v>
+        <v>86.131900000000002</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="2" t="e">
+      <c r="E11" s="2">
         <f>STDEV(E5:E8)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F11" s="2" t="e">
+        <v>1.3576450198780218E-2</v>
+      </c>
+      <c r="F11" s="2">
         <f>STDEV(F5:F8)</f>
-        <v>#DIV/0!</v>
+        <v>0.13321891757554657</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -2786,7 +2878,7 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -2797,7 +2889,7 @@
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -2808,7 +2900,7 @@
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -2819,7 +2911,7 @@
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -2830,7 +2922,7 @@
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -2841,7 +2933,7 @@
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -2852,7 +2944,7 @@
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -2863,7 +2955,7 @@
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -2874,7 +2966,7 @@
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -2885,7 +2977,7 @@
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -2896,7 +2988,7 @@
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -2907,7 +2999,7 @@
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -2918,7 +3010,7 @@
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -2929,7 +3021,7 @@
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -2940,7 +3032,7 @@
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -2951,7 +3043,7 @@
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -2962,7 +3054,7 @@
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -2973,7 +3065,7 @@
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>

</xml_diff>

<commit_message>
första 3 GAT 4l pnorm :rocket:
</commit_message>
<xml_diff>
--- a/Resultat/Resultat.xlsx
+++ b/Resultat/Resultat.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B70725-3F7C-3948-8F9D-0A3A5EDEC7F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="6_{7039940C-286B-48B0-BE5E-FEEB92B7113D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{CB7C2BC5-74E7-43ED-BB0A-E4ED42944523}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="21600" windowHeight="11380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13425" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GATED" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="56">
   <si>
     <t>SEED</t>
   </si>
@@ -185,6 +185,18 @@
   </si>
   <si>
     <t>6213.1886</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P-norm, nn.Parameter(torch.rand(out_dim)*3+1) , torch.clamp(self.p,1,100), PATTERN, </t>
+  </si>
+  <si>
+    <t>P100</t>
+  </si>
+  <si>
+    <t>Ej klar</t>
+  </si>
+  <si>
+    <t>V100</t>
   </si>
 </sst>
 </file>
@@ -747,36 +759,36 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Tabell2112" displayName="Tabell2112" ref="B4:J11" totalsRowShown="0" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Tabell2112" displayName="Tabell2112" ref="B4:J11" totalsRowShown="0" dataDxfId="29">
   <autoFilter ref="B4:J11" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="SEED" dataDxfId="18"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0900-00000C000000}" name="Layers" dataDxfId="17"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0900-00000A000000}" name="Params" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="TEST_ACC" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="TRAIN_ACC" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="EPOCHS" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="EPOCH TIME" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0900-000006000000}" name="TOTAL TIME (s)" dataDxfId="11"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0900-00000B000000}" name="GPU" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="SEED" dataDxfId="28"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0900-00000C000000}" name="Layers" dataDxfId="27"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0900-00000A000000}" name="Params" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="TEST_ACC" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="TRAIN_ACC" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="EPOCHS" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="EPOCH TIME" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0900-000006000000}" name="TOTAL TIME (s)" dataDxfId="21"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0900-00000B000000}" name="GPU" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="Tabell21123" displayName="Tabell21123" ref="B14:J21" totalsRowShown="0" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="Tabell21123" displayName="Tabell21123" ref="B14:J21" totalsRowShown="0" dataDxfId="19">
   <autoFilter ref="B14:J21" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="SEED" dataDxfId="8"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0A00-00000C000000}" name="Layers" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0A00-00000A000000}" name="Params" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="TEST_ACC" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0A00-000003000000}" name="TRAIN_ACC" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0A00-000004000000}" name="EPOCHS" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0A00-000005000000}" name="EPOCH TIME" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0A00-000006000000}" name="TOTAL TIME (h)" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0A00-00000B000000}" name="GPU" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="SEED" dataDxfId="18"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0A00-00000C000000}" name="Layers" dataDxfId="17"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0A00-00000A000000}" name="Params" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="TEST_ACC" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0A00-000003000000}" name="TRAIN_ACC" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0A00-000004000000}" name="EPOCHS" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0A00-000005000000}" name="EPOCH TIME" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0A00-000006000000}" name="TOTAL TIME (h)" dataDxfId="11"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0A00-00000B000000}" name="GPU" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -909,18 +921,18 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="32" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Tabell2112433" displayName="Tabell2112433" ref="C37:K46" totalsRowShown="0" dataDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="32" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Tabell2112433" displayName="Tabell2112433" ref="C37:K46" totalsRowShown="0" dataDxfId="9">
   <autoFilter ref="C37:K46" xr:uid="{00000000-0009-0000-0100-000020000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="SEED" dataDxfId="28"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0800-00000C000000}" name="Layers" dataDxfId="27"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0800-00000A000000}" name="Params" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="TEST_ACC" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="TRAIN_ACC" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="EPOCHS" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="EPOCH TIME" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="TOTAL TIME" dataDxfId="21"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0800-00000B000000}" name="GPU" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="SEED" dataDxfId="8"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0800-00000C000000}" name="Layers" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0800-00000A000000}" name="Params" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="TEST_ACC" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="TRAIN_ACC" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="EPOCHS" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="EPOCH TIME" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="TOTAL TIME" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0800-00000B000000}" name="GPU" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1253,31 +1265,31 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="13.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" customWidth="1"/>
+    <col min="3" max="3" width="15.1328125" customWidth="1"/>
+    <col min="4" max="4" width="12.1328125" customWidth="1"/>
     <col min="5" max="5" width="15.6640625" customWidth="1"/>
     <col min="6" max="6" width="18.33203125" customWidth="1"/>
-    <col min="7" max="7" width="14.83203125" customWidth="1"/>
-    <col min="8" max="8" width="17.1640625" customWidth="1"/>
-    <col min="9" max="9" width="17.5" customWidth="1"/>
-    <col min="10" max="10" width="19.5" customWidth="1"/>
+    <col min="7" max="7" width="14.796875" customWidth="1"/>
+    <col min="8" max="8" width="17.1328125" customWidth="1"/>
+    <col min="9" max="9" width="17.46484375" customWidth="1"/>
+    <col min="10" max="10" width="19.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B4" s="6" t="s">
         <v>0</v>
       </c>
@@ -1306,7 +1318,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B5" s="7">
         <v>41</v>
       </c>
@@ -1335,7 +1347,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B6" s="7">
         <v>35</v>
       </c>
@@ -1364,7 +1376,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B7" s="7">
         <v>12</v>
       </c>
@@ -1393,7 +1405,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B8" s="7">
         <v>95</v>
       </c>
@@ -1422,7 +1434,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -1433,7 +1445,7 @@
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
@@ -1444,7 +1456,7 @@
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
@@ -1455,7 +1467,7 @@
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" s="4" t="s">
         <v>21</v>
       </c>
@@ -1475,7 +1487,7 @@
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
@@ -1492,12 +1504,12 @@
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
         <v>0</v>
       </c>
@@ -1526,7 +1538,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -1537,7 +1549,7 @@
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -1548,7 +1560,7 @@
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -1559,7 +1571,7 @@
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -1570,7 +1582,7 @@
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -1581,7 +1593,7 @@
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -1592,7 +1604,7 @@
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -1603,7 +1615,7 @@
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -1614,7 +1626,7 @@
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -1625,12 +1637,12 @@
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B35" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B36" t="s">
         <v>0</v>
       </c>
@@ -1659,7 +1671,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -1670,7 +1682,7 @@
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -1681,7 +1693,7 @@
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -1692,7 +1704,7 @@
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -1703,7 +1715,7 @@
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -1714,7 +1726,7 @@
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -1725,7 +1737,7 @@
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -1736,7 +1748,7 @@
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -1747,7 +1759,7 @@
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -1773,24 +1785,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="M38" sqref="M38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="11.5" customWidth="1"/>
-    <col min="3" max="3" width="13.5" customWidth="1"/>
+    <col min="2" max="2" width="11.46484375" customWidth="1"/>
+    <col min="3" max="3" width="13.46484375" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.1640625" customWidth="1"/>
+    <col min="5" max="5" width="14.796875" customWidth="1"/>
+    <col min="6" max="6" width="12.1328125" customWidth="1"/>
     <col min="7" max="7" width="11.33203125" customWidth="1"/>
-    <col min="8" max="8" width="13.5" customWidth="1"/>
-    <col min="9" max="9" width="19.83203125" customWidth="1"/>
+    <col min="8" max="8" width="13.46484375" customWidth="1"/>
+    <col min="9" max="9" width="19.796875" customWidth="1"/>
     <col min="10" max="10" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
         <v>12</v>
       </c>
@@ -1816,12 +1828,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -1850,7 +1862,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="B5" s="2">
         <v>41</v>
       </c>
@@ -1880,7 +1892,7 @@
       </c>
       <c r="N5" s="1"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="B6" s="2">
         <v>53</v>
       </c>
@@ -1909,7 +1921,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="B7" s="2">
         <v>76</v>
       </c>
@@ -1938,7 +1950,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="B8" s="2">
         <v>12</v>
       </c>
@@ -1967,7 +1979,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -1978,7 +1990,7 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="s">
         <v>21</v>
       </c>
@@ -1998,7 +2010,7 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -2015,7 +2027,7 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -2026,7 +2038,7 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -2037,12 +2049,12 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
         <v>0</v>
       </c>
@@ -2071,7 +2083,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B21" s="2">
         <v>41</v>
       </c>
@@ -2100,7 +2112,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B22" s="2">
         <v>95</v>
       </c>
@@ -2129,7 +2141,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B23" s="2">
         <v>12</v>
       </c>
@@ -2158,7 +2170,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B24" s="2">
         <v>35</v>
       </c>
@@ -2187,7 +2199,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -2198,7 +2210,7 @@
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -2209,7 +2221,7 @@
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -2220,7 +2232,7 @@
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A28" s="4" t="s">
         <v>21</v>
       </c>
@@ -2240,7 +2252,7 @@
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -2257,7 +2269,7 @@
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B34" t="s">
         <v>47</v>
       </c>
@@ -2286,12 +2298,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B35" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B36" t="s">
         <v>0</v>
       </c>
@@ -2320,7 +2332,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B37" s="2">
         <v>41</v>
       </c>
@@ -2349,7 +2361,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B38" s="2">
         <v>95</v>
       </c>
@@ -2364,7 +2376,7 @@
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B39" s="2">
         <v>12</v>
       </c>
@@ -2379,7 +2391,7 @@
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B40" s="2">
         <v>35</v>
       </c>
@@ -2394,7 +2406,7 @@
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -2405,7 +2417,7 @@
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -2416,7 +2428,7 @@
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -2427,7 +2439,7 @@
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -2438,7 +2450,7 @@
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -2462,20 +2474,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="C4:K46"/>
+  <dimension ref="C4:L46"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="J48" sqref="J48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="4" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C5" t="s">
         <v>0</v>
       </c>
@@ -2504,7 +2516,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -2515,7 +2527,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -2526,7 +2538,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -2537,7 +2549,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -2548,7 +2560,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -2559,7 +2571,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -2570,7 +2582,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -2581,7 +2593,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -2592,7 +2604,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -2603,12 +2615,12 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="20" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C20" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C21" t="s">
         <v>0</v>
       </c>
@@ -2637,7 +2649,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -2648,7 +2660,7 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -2659,7 +2671,7 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -2670,7 +2682,7 @@
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -2681,7 +2693,7 @@
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -2692,7 +2704,7 @@
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -2703,7 +2715,7 @@
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -2714,7 +2726,7 @@
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
     </row>
-    <row r="29" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -2725,7 +2737,7 @@
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -2736,12 +2748,12 @@
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
     </row>
-    <row r="36" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="3:12" x14ac:dyDescent="0.45">
       <c r="C36" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="3:11" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="3:12" x14ac:dyDescent="0.45">
       <c r="C37" t="s">
         <v>0</v>
       </c>
@@ -2770,51 +2782,116 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
-      <c r="K38" s="2"/>
-    </row>
-    <row r="39" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
-      <c r="K39" s="2"/>
-    </row>
-    <row r="40" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
-    </row>
-    <row r="41" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
+    <row r="38" spans="3:12" x14ac:dyDescent="0.45">
+      <c r="C38" s="2">
+        <v>41</v>
+      </c>
+      <c r="D38" s="2">
+        <v>4</v>
+      </c>
+      <c r="E38" s="2">
+        <v>110540</v>
+      </c>
+      <c r="F38" s="2">
+        <v>85.662999999999997</v>
+      </c>
+      <c r="G38" s="2">
+        <v>86.120500000000007</v>
+      </c>
+      <c r="H38" s="2">
+        <v>63</v>
+      </c>
+      <c r="I38" s="2">
+        <v>382.9778</v>
+      </c>
+      <c r="J38" s="2">
+        <v>24661.905999999999</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="3:12" x14ac:dyDescent="0.45">
+      <c r="C39" s="2">
+        <v>35</v>
+      </c>
+      <c r="D39" s="2">
+        <v>4</v>
+      </c>
+      <c r="E39" s="2">
+        <v>110540</v>
+      </c>
+      <c r="F39" s="2">
+        <v>85.691999999999993</v>
+      </c>
+      <c r="G39" s="2">
+        <v>86.033900000000003</v>
+      </c>
+      <c r="H39" s="2">
+        <v>57</v>
+      </c>
+      <c r="I39" s="2">
+        <v>386.4939</v>
+      </c>
+      <c r="J39" s="2">
+        <v>22573.454300000001</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="40" spans="3:12" x14ac:dyDescent="0.45">
+      <c r="C40" s="2">
+        <v>12</v>
+      </c>
+      <c r="D40" s="2">
+        <v>4</v>
+      </c>
+      <c r="E40" s="2">
+        <v>110540</v>
+      </c>
+      <c r="F40" s="2">
+        <v>85.64</v>
+      </c>
+      <c r="G40" s="2">
+        <v>85.933300000000003</v>
+      </c>
+      <c r="H40" s="2">
+        <v>59</v>
+      </c>
+      <c r="I40" s="2">
+        <v>288.84780000000001</v>
+      </c>
+      <c r="J40" s="2">
+        <v>23492.045300000002</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="41" spans="3:12" x14ac:dyDescent="0.45">
+      <c r="C41" s="2">
+        <v>95</v>
+      </c>
+      <c r="D41" s="2">
+        <v>4</v>
+      </c>
+      <c r="E41" s="2">
+        <v>110540</v>
+      </c>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
-    </row>
-    <row r="42" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="K41" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="L41" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="42" spans="3:12" x14ac:dyDescent="0.45">
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -2825,7 +2902,7 @@
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
     </row>
-    <row r="43" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="3:12" x14ac:dyDescent="0.45">
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -2836,7 +2913,7 @@
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
     </row>
-    <row r="44" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="3:12" x14ac:dyDescent="0.45">
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -2847,7 +2924,7 @@
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
     </row>
-    <row r="45" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="3:12" x14ac:dyDescent="0.45">
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -2858,7 +2935,7 @@
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
     </row>
-    <row r="46" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="3:12" x14ac:dyDescent="0.45">
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
@@ -2871,10 +2948,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <tableParts count="3">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2883,23 +2961,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="3" width="11.33203125" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" customWidth="1"/>
     <col min="5" max="5" width="14.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.1640625" customWidth="1"/>
-    <col min="7" max="7" width="10.5" customWidth="1"/>
-    <col min="8" max="8" width="15.5" customWidth="1"/>
+    <col min="6" max="6" width="13.1328125" customWidth="1"/>
+    <col min="7" max="7" width="10.46484375" customWidth="1"/>
+    <col min="8" max="8" width="15.46484375" customWidth="1"/>
     <col min="9" max="9" width="16.6640625" customWidth="1"/>
-    <col min="10" max="10" width="17.1640625" customWidth="1"/>
+    <col min="10" max="10" width="17.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
         <v>12</v>
       </c>
@@ -2926,16 +3004,16 @@
       </c>
       <c r="L1" s="5"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="L2" s="5"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>45</v>
       </c>
       <c r="L3" s="5"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -2965,7 +3043,7 @@
       </c>
       <c r="L4" s="5"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B5" s="2">
         <v>41</v>
       </c>
@@ -2994,7 +3072,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B6" s="2">
         <v>95</v>
       </c>
@@ -3023,7 +3101,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B7" s="2">
         <v>12</v>
       </c>
@@ -3052,7 +3130,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B8" s="2">
         <v>35</v>
       </c>
@@ -3081,7 +3159,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -3092,7 +3170,7 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="s">
         <v>21</v>
       </c>
@@ -3112,7 +3190,7 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -3129,7 +3207,7 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -3140,12 +3218,12 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
         <v>0</v>
       </c>
@@ -3174,7 +3252,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B15" s="2">
         <v>41</v>
       </c>
@@ -3203,7 +3281,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B16" s="2">
         <v>95</v>
       </c>
@@ -3220,7 +3298,7 @@
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B17" s="2">
         <v>12</v>
       </c>
@@ -3235,7 +3313,7 @@
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B18" s="2">
         <v>35</v>
       </c>
@@ -3250,7 +3328,7 @@
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -3261,7 +3339,7 @@
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" s="4" t="s">
         <v>21</v>
       </c>
@@ -3281,7 +3359,7 @@
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -3298,7 +3376,7 @@
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -3309,7 +3387,7 @@
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -3320,7 +3398,7 @@
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -3331,7 +3409,7 @@
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -3342,7 +3420,7 @@
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -3353,7 +3431,7 @@
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -3364,7 +3442,7 @@
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -3375,7 +3453,7 @@
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -3386,7 +3464,7 @@
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -3397,7 +3475,7 @@
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -3408,7 +3486,7 @@
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -3419,7 +3497,7 @@
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -3430,7 +3508,7 @@
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -3441,7 +3519,7 @@
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -3452,7 +3530,7 @@
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -3463,7 +3541,7 @@
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>

</xml_diff>

<commit_message>
GAT pnorm 4l klar :rocket:
</commit_message>
<xml_diff>
--- a/Resultat/Resultat.xlsx
+++ b/Resultat/Resultat.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="46" documentId="6_{7039940C-286B-48B0-BE5E-FEEB92B7113D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{CB7C2BC5-74E7-43ED-BB0A-E4ED42944523}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="6_{7039940C-286B-48B0-BE5E-FEEB92B7113D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8B2F23B2-3028-4B53-B1C8-FD172B8D40BE}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13425" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="55">
   <si>
     <t>SEED</t>
   </si>
@@ -193,10 +193,7 @@
     <t>P100</t>
   </si>
   <si>
-    <t>Ej klar</t>
-  </si>
-  <si>
-    <t>V100</t>
+    <t>5.6268h</t>
   </si>
 </sst>
 </file>
@@ -206,7 +203,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,6 +235,18 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -265,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -289,6 +298,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -759,36 +774,36 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Tabell2112" displayName="Tabell2112" ref="B4:J11" totalsRowShown="0" dataDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Tabell2112" displayName="Tabell2112" ref="B4:J11" totalsRowShown="0" dataDxfId="19">
   <autoFilter ref="B4:J11" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="SEED" dataDxfId="28"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0900-00000C000000}" name="Layers" dataDxfId="27"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0900-00000A000000}" name="Params" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="TEST_ACC" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="TRAIN_ACC" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="EPOCHS" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="EPOCH TIME" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0900-000006000000}" name="TOTAL TIME (s)" dataDxfId="21"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0900-00000B000000}" name="GPU" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="SEED" dataDxfId="18"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0900-00000C000000}" name="Layers" dataDxfId="17"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0900-00000A000000}" name="Params" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="TEST_ACC" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="TRAIN_ACC" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="EPOCHS" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="EPOCH TIME" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0900-000006000000}" name="TOTAL TIME (s)" dataDxfId="11"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0900-00000B000000}" name="GPU" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="Tabell21123" displayName="Tabell21123" ref="B14:J21" totalsRowShown="0" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="Tabell21123" displayName="Tabell21123" ref="B14:J21" totalsRowShown="0" dataDxfId="9">
   <autoFilter ref="B14:J21" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="SEED" dataDxfId="18"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0A00-00000C000000}" name="Layers" dataDxfId="17"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0A00-00000A000000}" name="Params" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="TEST_ACC" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0A00-000003000000}" name="TRAIN_ACC" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0A00-000004000000}" name="EPOCHS" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0A00-000005000000}" name="EPOCH TIME" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0A00-000006000000}" name="TOTAL TIME (h)" dataDxfId="11"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0A00-00000B000000}" name="GPU" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="SEED" dataDxfId="8"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0A00-00000C000000}" name="Layers" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0A00-00000A000000}" name="Params" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="TEST_ACC" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0A00-000003000000}" name="TRAIN_ACC" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0A00-000004000000}" name="EPOCHS" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0A00-000005000000}" name="EPOCH TIME" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0A00-000006000000}" name="TOTAL TIME (h)" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0A00-00000B000000}" name="GPU" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -921,18 +936,18 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="32" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Tabell2112433" displayName="Tabell2112433" ref="C37:K46" totalsRowShown="0" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="32" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Tabell2112433" displayName="Tabell2112433" ref="C37:K46" totalsRowShown="0" dataDxfId="29">
   <autoFilter ref="C37:K46" xr:uid="{00000000-0009-0000-0100-000020000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="SEED" dataDxfId="8"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0800-00000C000000}" name="Layers" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0800-00000A000000}" name="Params" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="TEST_ACC" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="TRAIN_ACC" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="EPOCHS" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="EPOCH TIME" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="TOTAL TIME" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0800-00000B000000}" name="GPU" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="SEED" dataDxfId="28"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0800-00000C000000}" name="Layers" dataDxfId="27"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0800-00000A000000}" name="Params" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="TEST_ACC" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="TRAIN_ACC" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="EPOCHS" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="EPOCH TIME" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="TOTAL TIME" dataDxfId="21"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0800-00000B000000}" name="GPU" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2474,10 +2489,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="C4:L46"/>
+  <dimension ref="C4:K46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="J48" sqref="J48"/>
+      <selection activeCell="O39" sqref="O39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2748,12 +2763,12 @@
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
     </row>
-    <row r="36" spans="3:12" x14ac:dyDescent="0.45">
+    <row r="36" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C36" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="3:12" x14ac:dyDescent="0.45">
+    <row r="37" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C37" t="s">
         <v>0</v>
       </c>
@@ -2782,7 +2797,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="3:12" x14ac:dyDescent="0.45">
+    <row r="38" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C38" s="2">
         <v>41</v>
       </c>
@@ -2811,7 +2826,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="3:12" x14ac:dyDescent="0.45">
+    <row r="39" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C39" s="2">
         <v>35</v>
       </c>
@@ -2840,7 +2855,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="40" spans="3:12" x14ac:dyDescent="0.45">
+    <row r="40" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C40" s="2">
         <v>12</v>
       </c>
@@ -2869,7 +2884,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="41" spans="3:12" x14ac:dyDescent="0.45">
+    <row r="41" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C41" s="2">
         <v>95</v>
       </c>
@@ -2879,19 +2894,26 @@
       <c r="E41" s="2">
         <v>110540</v>
       </c>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
+      <c r="F41" s="11">
+        <v>85.686099999999996</v>
+      </c>
+      <c r="G41" s="12">
+        <v>85.858500000000006</v>
+      </c>
+      <c r="H41" s="2">
+        <v>51</v>
+      </c>
+      <c r="I41" s="12">
+        <v>386.565</v>
+      </c>
+      <c r="J41" s="11" t="s">
+        <v>54</v>
+      </c>
       <c r="K41" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="L41" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="42" spans="3:12" x14ac:dyDescent="0.45">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="42" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -2902,7 +2924,7 @@
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
     </row>
-    <row r="43" spans="3:12" x14ac:dyDescent="0.45">
+    <row r="43" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -2913,7 +2935,7 @@
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
     </row>
-    <row r="44" spans="3:12" x14ac:dyDescent="0.45">
+    <row r="44" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -2924,7 +2946,7 @@
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
     </row>
-    <row r="45" spans="3:12" x14ac:dyDescent="0.45">
+    <row r="45" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -2935,7 +2957,7 @@
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
     </row>
-    <row r="46" spans="3:12" x14ac:dyDescent="0.45">
+    <row r="46" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>

</xml_diff>